<commit_message>
Master Installment Commit by Arvind
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/uiAutomation/data/FeeModueData.xlsx
+++ b/src/main/java/com/test/automation/uiAutomation/data/FeeModueData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="FeeGroupMasterData" sheetId="1" r:id="rId1"/>
@@ -15,46 +15,47 @@
     <sheet name="Search_FeeHeadData" sheetId="41" r:id="rId6"/>
     <sheet name="FeeMasterInstallmentData" sheetId="4" r:id="rId7"/>
     <sheet name="FeeMasterInstallmentName" sheetId="5" r:id="rId8"/>
-    <sheet name="InstallmentDueDateData" sheetId="6" r:id="rId9"/>
-    <sheet name="YearlyGrHeadMap" sheetId="7" r:id="rId10"/>
-    <sheet name="YGHMFeeHeadInstallment" sheetId="8" r:id="rId11"/>
-    <sheet name="FeeLoginPreviledge" sheetId="9" r:id="rId12"/>
-    <sheet name="studentFeeGroupTestData" sheetId="10" r:id="rId13"/>
-    <sheet name="FeeTransactionStuName" sheetId="11" r:id="rId14"/>
-    <sheet name="FTransStudentInfoData" sheetId="12" r:id="rId15"/>
-    <sheet name="FeeTransFeeHeadAmont" sheetId="13" r:id="rId16"/>
-    <sheet name="BankDetailsData" sheetId="14" r:id="rId17"/>
-    <sheet name="FeeTermMasterData" sheetId="15" r:id="rId18"/>
-    <sheet name="FeeTermMasterEditData" sheetId="16" r:id="rId19"/>
-    <sheet name="FeesTermFeesHeadData" sheetId="17" r:id="rId20"/>
-    <sheet name="FeeHeadForFeeTermData" sheetId="18" r:id="rId21"/>
-    <sheet name="FeeCategoryNameCodeData" sheetId="19" r:id="rId22"/>
-    <sheet name="SearchByCCategoryName" sheetId="20" r:id="rId23"/>
-    <sheet name="YearlyClassCategoryData" sheetId="21" r:id="rId24"/>
-    <sheet name="CustomFeeGroupData" sheetId="22" r:id="rId25"/>
-    <sheet name="CreatedCustomNameData" sheetId="23" r:id="rId26"/>
-    <sheet name="FeeItReceiptData" sheetId="24" r:id="rId27"/>
-    <sheet name="CustomSPlFeeHeadData" sheetId="25" r:id="rId28"/>
-    <sheet name="CustomSplFeeHeadNameData" sheetId="26" r:id="rId29"/>
-    <sheet name="MasterFineSlabBetweenData" sheetId="27" r:id="rId30"/>
-    <sheet name="MasterFineSlabGreater&amp;LThanData" sheetId="28" r:id="rId31"/>
-    <sheet name="ToDAYFineSlab" sheetId="29" r:id="rId32"/>
-    <sheet name="FromDAYFineSlab" sheetId="30" r:id="rId33"/>
-    <sheet name="FeeAmountEntryData" sheetId="31" r:id="rId34"/>
-    <sheet name="InstallmentIData" sheetId="32" r:id="rId35"/>
-    <sheet name="FeeSlabPopUpDetails" sheetId="33" r:id="rId36"/>
-    <sheet name="InstallmentIIData" sheetId="34" r:id="rId37"/>
-    <sheet name="InstallmentIIIData" sheetId="35" r:id="rId38"/>
-    <sheet name="InstallmentIVData" sheetId="36" r:id="rId39"/>
-    <sheet name="InstallmentVData" sheetId="37" r:id="rId40"/>
-    <sheet name="SearchAndDeleteTestData" sheetId="38" r:id="rId41"/>
+    <sheet name="Search_MasterInstallmentName" sheetId="42" r:id="rId9"/>
+    <sheet name="InstallmentDueDateData" sheetId="6" r:id="rId10"/>
+    <sheet name="YearlyGrHeadMap" sheetId="7" r:id="rId11"/>
+    <sheet name="YGHMFeeHeadInstallment" sheetId="8" r:id="rId12"/>
+    <sheet name="FeeLoginPreviledge" sheetId="9" r:id="rId13"/>
+    <sheet name="studentFeeGroupTestData" sheetId="10" r:id="rId14"/>
+    <sheet name="FeeTransactionStuName" sheetId="11" r:id="rId15"/>
+    <sheet name="FTransStudentInfoData" sheetId="12" r:id="rId16"/>
+    <sheet name="FeeTransFeeHeadAmont" sheetId="13" r:id="rId17"/>
+    <sheet name="BankDetailsData" sheetId="14" r:id="rId18"/>
+    <sheet name="FeeTermMasterData" sheetId="15" r:id="rId19"/>
+    <sheet name="FeeTermMasterEditData" sheetId="16" r:id="rId20"/>
+    <sheet name="FeesTermFeesHeadData" sheetId="17" r:id="rId21"/>
+    <sheet name="FeeHeadForFeeTermData" sheetId="18" r:id="rId22"/>
+    <sheet name="FeeCategoryNameCodeData" sheetId="19" r:id="rId23"/>
+    <sheet name="SearchByCCategoryName" sheetId="20" r:id="rId24"/>
+    <sheet name="YearlyClassCategoryData" sheetId="21" r:id="rId25"/>
+    <sheet name="CustomFeeGroupData" sheetId="22" r:id="rId26"/>
+    <sheet name="CreatedCustomNameData" sheetId="23" r:id="rId27"/>
+    <sheet name="FeeItReceiptData" sheetId="24" r:id="rId28"/>
+    <sheet name="CustomSPlFeeHeadData" sheetId="25" r:id="rId29"/>
+    <sheet name="CustomSplFeeHeadNameData" sheetId="26" r:id="rId30"/>
+    <sheet name="MasterFineSlabBetweenData" sheetId="27" r:id="rId31"/>
+    <sheet name="MasterFineSlabGreater&amp;LThanData" sheetId="28" r:id="rId32"/>
+    <sheet name="ToDAYFineSlab" sheetId="29" r:id="rId33"/>
+    <sheet name="FromDAYFineSlab" sheetId="30" r:id="rId34"/>
+    <sheet name="FeeAmountEntryData" sheetId="31" r:id="rId35"/>
+    <sheet name="InstallmentIData" sheetId="32" r:id="rId36"/>
+    <sheet name="FeeSlabPopUpDetails" sheetId="33" r:id="rId37"/>
+    <sheet name="InstallmentIIData" sheetId="34" r:id="rId38"/>
+    <sheet name="InstallmentIIIData" sheetId="35" r:id="rId39"/>
+    <sheet name="InstallmentIVData" sheetId="36" r:id="rId40"/>
+    <sheet name="InstallmentVData" sheetId="37" r:id="rId41"/>
+    <sheet name="SearchAndDeleteTestData" sheetId="38" r:id="rId42"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="150">
   <si>
     <t>Group Name</t>
   </si>
@@ -1037,21 +1038,21 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1061,6 +1062,48 @@
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
@@ -1074,7 +1117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1126,7 +1169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1188,7 +1231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1230,7 +1273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1265,7 +1308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1375,7 +1418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1411,7 +1454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1467,7 +1510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1510,7 +1553,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1544,45 +1625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1624,7 +1667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1658,7 +1701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1711,7 +1754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1753,7 +1796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1816,7 +1859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1879,7 +1922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1921,7 +1964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1983,7 +2026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2035,7 +2078,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2078,60 +2174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2179,7 +2222,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2232,7 +2275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2267,7 +2310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2302,7 +2345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2350,7 +2393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2403,7 +2446,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2446,7 +2489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2499,7 +2542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2552,7 +2595,41 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2605,41 +2682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2693,7 +2736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2773,7 +2816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2917,42 +2960,35 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit Student fee group changes
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/uiAutomation/data/FeeModueData.xlsx
+++ b/src/main/java/com/test/automation/uiAutomation/data/FeeModueData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" firstSheet="46" activeTab="47"/>
   </bookViews>
   <sheets>
     <sheet name="FeeGroupMasterData" sheetId="1" r:id="rId1"/>
@@ -21,42 +21,47 @@
     <sheet name="YearlyGrHeadMap" sheetId="7" r:id="rId12"/>
     <sheet name="YGHMFeeHeadInstallment" sheetId="8" r:id="rId13"/>
     <sheet name="FeeLoginPreviledge" sheetId="9" r:id="rId14"/>
-    <sheet name="studentFeeGroupTestData" sheetId="10" r:id="rId15"/>
-    <sheet name="FeeTransactionStuName" sheetId="11" r:id="rId16"/>
-    <sheet name="FTransStudentInfoData" sheetId="12" r:id="rId17"/>
-    <sheet name="FeeTransFeeHeadAmont" sheetId="13" r:id="rId18"/>
-    <sheet name="BankDetailsData" sheetId="14" r:id="rId19"/>
-    <sheet name="FeeTermMasterData" sheetId="15" r:id="rId20"/>
-    <sheet name="FeeTermMasterEditData" sheetId="16" r:id="rId21"/>
-    <sheet name="FeesTermFeesHeadData" sheetId="17" r:id="rId22"/>
-    <sheet name="FeeHeadForFeeTermData" sheetId="18" r:id="rId23"/>
-    <sheet name="FeeCategoryNameCodeData" sheetId="19" r:id="rId24"/>
-    <sheet name="SearchByCCategoryName" sheetId="20" r:id="rId25"/>
-    <sheet name="YearlyClassCategoryData" sheetId="21" r:id="rId26"/>
-    <sheet name="CustomFeeGroupData" sheetId="22" r:id="rId27"/>
-    <sheet name="CreatedCustomNameData" sheetId="23" r:id="rId28"/>
-    <sheet name="FeeItReceiptData" sheetId="24" r:id="rId29"/>
-    <sheet name="CustomSPlFeeHeadData" sheetId="25" r:id="rId30"/>
-    <sheet name="Search_CustomSplFeeHead" sheetId="26" r:id="rId31"/>
-    <sheet name="MasterFineSlabBetweenData" sheetId="27" r:id="rId32"/>
-    <sheet name="MasterFineSlabGreater&amp;LThanData" sheetId="28" r:id="rId33"/>
-    <sheet name="ToDAYFineSlab" sheetId="29" r:id="rId34"/>
-    <sheet name="FromDAYFineSlab" sheetId="30" r:id="rId35"/>
-    <sheet name="FeeAmountEntryData" sheetId="31" r:id="rId36"/>
-    <sheet name="InstallmentIData" sheetId="32" r:id="rId37"/>
-    <sheet name="FeeSlabPopUpDetails" sheetId="33" r:id="rId38"/>
-    <sheet name="InstallmentIIData" sheetId="34" r:id="rId39"/>
-    <sheet name="InstallmentIIIData" sheetId="35" r:id="rId40"/>
-    <sheet name="InstallmentIVData" sheetId="36" r:id="rId41"/>
-    <sheet name="InstallmentVData" sheetId="37" r:id="rId42"/>
-    <sheet name="SearchAndDeleteTestData" sheetId="38" r:id="rId43"/>
+    <sheet name="FeeTransactionStuName" sheetId="11" r:id="rId15"/>
+    <sheet name="FTransStudentInfoData" sheetId="12" r:id="rId16"/>
+    <sheet name="FeeTransFeeHeadAmont" sheetId="13" r:id="rId17"/>
+    <sheet name="BankDetailsData" sheetId="14" r:id="rId18"/>
+    <sheet name="FeeTermMasterData" sheetId="15" r:id="rId19"/>
+    <sheet name="FeeTermMasterEditData" sheetId="16" r:id="rId20"/>
+    <sheet name="FeesTermFeesHeadData" sheetId="17" r:id="rId21"/>
+    <sheet name="FeeHeadForFeeTermData" sheetId="18" r:id="rId22"/>
+    <sheet name="FeeCategoryNameCodeData" sheetId="19" r:id="rId23"/>
+    <sheet name="SearchByCCategoryName" sheetId="20" r:id="rId24"/>
+    <sheet name="YearlyClassCategoryData" sheetId="21" r:id="rId25"/>
+    <sheet name="CustomFeeGroupData" sheetId="22" r:id="rId26"/>
+    <sheet name="CreatedCustomNameData" sheetId="23" r:id="rId27"/>
+    <sheet name="FeeItReceiptData" sheetId="24" r:id="rId28"/>
+    <sheet name="CustomSPlFeeHeadData" sheetId="25" r:id="rId29"/>
+    <sheet name="Search_CustomSplFeeHead" sheetId="26" r:id="rId30"/>
+    <sheet name="MasterFineSlabBetweenData" sheetId="27" r:id="rId31"/>
+    <sheet name="MasterFineSlabGreater&amp;LThanData" sheetId="28" r:id="rId32"/>
+    <sheet name="ToDAYFineSlab" sheetId="29" r:id="rId33"/>
+    <sheet name="FromDAYFineSlab" sheetId="30" r:id="rId34"/>
+    <sheet name="FeeAmountEntryData" sheetId="31" r:id="rId35"/>
+    <sheet name="InstallmentIData" sheetId="32" r:id="rId36"/>
+    <sheet name="FeeSlabPopUpDetails" sheetId="33" r:id="rId37"/>
+    <sheet name="InstallmentIIData" sheetId="34" r:id="rId38"/>
+    <sheet name="InstallmentIIIData" sheetId="35" r:id="rId39"/>
+    <sheet name="InstallmentIVData" sheetId="36" r:id="rId40"/>
+    <sheet name="InstallmentVData" sheetId="37" r:id="rId41"/>
+    <sheet name="SearchAndDeleteTestData" sheetId="38" r:id="rId42"/>
+    <sheet name="StudentFeeGrMap_wOutCLassWise" sheetId="44" r:id="rId43"/>
+    <sheet name="StudentFeeGrMap_withCLassWise" sheetId="45" r:id="rId44"/>
+    <sheet name="StudentFeeGrMap_FCCategory" sheetId="46" r:id="rId45"/>
+    <sheet name="StudentFeeGrMap_AdmCategory" sheetId="47" r:id="rId46"/>
+    <sheet name="Search_SFGMap_wOutCLassWise" sheetId="48" r:id="rId47"/>
+    <sheet name="Search_SFGMap_withCLassWise" sheetId="49" r:id="rId48"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="163">
   <si>
     <t>Group Name</t>
   </si>
@@ -181,12 +186,6 @@
     <t>COORDINATOR</t>
   </si>
   <si>
-    <t>BystudentNameSearch</t>
-  </si>
-  <si>
-    <t>StudentToSearch</t>
-  </si>
-  <si>
     <t>Student Name</t>
   </si>
   <si>
@@ -469,9 +468,6 @@
     <t>Susdiny School Fee Term Edit</t>
   </si>
   <si>
-    <t>S NISARGA</t>
-  </si>
-  <si>
     <t>Susdiny Duplicate Fee Head</t>
   </si>
   <si>
@@ -530,18 +526,49 @@
   </si>
   <si>
     <t>Invoice 5</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Fee Class Category</t>
+  </si>
+  <si>
+    <t>Nursery</t>
+  </si>
+  <si>
+    <t>Admission Category</t>
+  </si>
+  <si>
+    <t>Kinder Garden</t>
+  </si>
+  <si>
+    <t>SearchFor</t>
+  </si>
+  <si>
+    <t>ARJUN R ARADHYA</t>
+  </si>
+  <si>
+    <t>AMOGH K KOUNDINYA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -631,18 +658,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -651,7 +675,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -669,24 +696,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1005,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1017,28 +1051,28 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>140</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D2" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B3" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
@@ -1085,7 +1119,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>17</v>
@@ -1114,10 +1148,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1277,7 +1311,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>40</v>
@@ -1293,7 +1327,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1301,54 +1335,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1356,7 +1348,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -1368,7 +1360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1389,28 +1381,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
@@ -1418,28 +1410,28 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>6</v>
@@ -1447,10 +1439,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3">
         <v>57</v>
@@ -1459,10 +1451,10 @@
         <v>9844098440</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="9">
@@ -1478,7 +1470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1497,12 +1489,12 @@
         <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3">
         <v>5500</v>
@@ -1514,7 +1506,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1532,16 +1524,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1549,16 +1541,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>72</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -1570,6 +1562,49 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
@@ -1594,14 +1629,14 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="16"/>
+      <c r="A3" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1610,20 +1645,20 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1631,17 +1666,50 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1651,98 +1719,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1761,7 +1753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1777,10 +1769,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1788,10 +1780,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -1799,10 +1791,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -1814,7 +1806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1829,7 +1821,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1837,7 +1829,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -1845,7 +1837,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
@@ -1856,7 +1848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1876,10 +1868,10 @@
         <v>30</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>2</v>
@@ -1890,10 +1882,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>4</v>
@@ -1904,10 +1896,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>6</v>
@@ -1919,7 +1911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1936,13 +1928,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1950,10 +1942,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -1964,10 +1956,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
@@ -1982,7 +1974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1997,7 +1989,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -2005,7 +1997,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -2013,7 +2005,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>6</v>
@@ -2024,7 +2016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2046,16 +2038,16 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -2066,18 +2058,70 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2141,88 +2185,36 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
-        <v>98</v>
+      <c r="A2" s="14" t="s">
+        <v>96</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="14" t="s">
-        <v>138</v>
+      <c r="A3" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
@@ -2230,7 +2222,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -2242,7 +2234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2259,13 +2251,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2273,14 +2265,14 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>105</v>
-      </c>
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
@@ -2290,7 +2282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2307,10 +2299,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -2318,25 +2310,60 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="10" t="s">
         <v>109</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -2348,12 +2375,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2380,41 +2407,6 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2433,7 +2425,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>31</v>
@@ -2447,7 +2439,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -2461,7 +2453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2477,16 +2469,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -2494,45 +2486,45 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="B1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2540,14 +2532,14 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>126</v>
-      </c>
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
@@ -2557,7 +2549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2573,16 +2565,69 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -2593,13 +2638,13 @@
         <v>127</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>128</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -2624,10 +2669,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2660,16 +2705,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -2680,13 +2725,13 @@
         <v>129</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>130</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -2702,27 +2747,28 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -2733,13 +2779,13 @@
         <v>131</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>132</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -2752,74 +2798,20 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -2827,7 +2819,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -2835,6 +2827,251 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2894,10 +3131,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2960,7 +3197,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -3037,20 +3274,20 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
@@ -3064,7 +3301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -3074,10 +3311,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3091,7 +3328,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Commit for Concession changes
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/uiAutomation/data/FeeModueData.xlsx
+++ b/src/main/java/com/test/automation/uiAutomation/data/FeeModueData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" firstSheet="46" activeTab="47"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" firstSheet="56" activeTab="56"/>
   </bookViews>
   <sheets>
     <sheet name="FeeGroupMasterData" sheetId="1" r:id="rId1"/>
@@ -53,15 +53,26 @@
     <sheet name="StudentFeeGrMap_withCLassWise" sheetId="45" r:id="rId44"/>
     <sheet name="StudentFeeGrMap_FCCategory" sheetId="46" r:id="rId45"/>
     <sheet name="StudentFeeGrMap_AdmCategory" sheetId="47" r:id="rId46"/>
-    <sheet name="Search_SFGMap_wOutCLassWise" sheetId="48" r:id="rId47"/>
-    <sheet name="Search_SFGMap_withCLassWise" sheetId="49" r:id="rId48"/>
+    <sheet name="SFGMap_wOutCLassWiseAll" sheetId="48" r:id="rId47"/>
+    <sheet name="SFGMap_withCLassWise_All" sheetId="49" r:id="rId48"/>
+    <sheet name="Search_SFGMap_FCCategory" sheetId="50" r:id="rId49"/>
+    <sheet name="Search_SFGMap_AdmCategory" sheetId="51" r:id="rId50"/>
+    <sheet name="SFGMap_RegStudent_woutClassWise" sheetId="52" r:id="rId51"/>
+    <sheet name="SFGMap_RegStudent_withClassWise" sheetId="53" r:id="rId52"/>
+    <sheet name="SFGMap_NewStudent_woutClassWise" sheetId="54" r:id="rId53"/>
+    <sheet name="SFGMap_NewStudent_withClassWise" sheetId="55" r:id="rId54"/>
+    <sheet name="FeeMasterConcession_ClassWise" sheetId="56" r:id="rId55"/>
+    <sheet name="FeeMasterConcession_CategoryWis" sheetId="57" r:id="rId56"/>
+    <sheet name="Search_FeeConc_Classwise" sheetId="58" r:id="rId57"/>
+    <sheet name="Search_FeeConc_CategoryWise" sheetId="59" r:id="rId58"/>
+    <sheet name="ConcessType_AndConcessionAmount" sheetId="60" r:id="rId59"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="175">
   <si>
     <t>Group Name</t>
   </si>
@@ -546,22 +557,72 @@
     <t>SearchFor</t>
   </si>
   <si>
-    <t>ARJUN R ARADHYA</t>
-  </si>
-  <si>
-    <t>AMOGH K KOUNDINYA</t>
+    <t>ARJUN R ARADHYA</t>
+  </si>
+  <si>
+    <t>ADITHYA A ATMA</t>
+  </si>
+  <si>
+    <t>AADYA S DARSHAN</t>
+  </si>
+  <si>
+    <t>KANISHKA RAM A</t>
+  </si>
+  <si>
+    <t>AISHWARYA KRATHU P</t>
+  </si>
+  <si>
+    <t>SIYON LESTER DSOUZA</t>
+  </si>
+  <si>
+    <t>KANISHKA RAM A</t>
+  </si>
+  <si>
+    <t>SAANVI SHENOY</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>NADI V KORAKOPPA</t>
+  </si>
+  <si>
+    <t>ConcessionType</t>
+  </si>
+  <si>
+    <t>Concession Amount</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>500</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -658,27 +719,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -696,28 +757,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -2835,7 +2905,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2853,7 +2923,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="10" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -2998,7 +3068,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3031,6 +3101,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3038,8 +3109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3064,6 +3135,48 @@
         <v>41</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>162</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -3114,6 +3227,411 @@
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="D4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>